<commit_message>
Update backlogs to match the github
</commit_message>
<xml_diff>
--- a/doc/QRChaserProductBacklog.xlsx
+++ b/doc/QRChaserProductBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\School\2021-22\CMPUT 301\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Davies\Documents\School Work\CMPUT301\QRChaser\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D25A47F-434A-4B9C-BC24-0024998CCE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE501D7-8853-4402-94A8-385C43C930C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D54E4526-E9DA-4E34-8655-911F54BBB230}"/>
+    <workbookView xWindow="3915" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{D54E4526-E9DA-4E34-8655-911F54BBB230}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="154">
   <si>
     <t>#</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Depracated</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Completed</t>
@@ -581,14 +578,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -907,8 +904,8 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,17 +939,17 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -963,19 +960,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>134</v>
-      </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -986,16 +983,16 @@
         <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1009,13 +1006,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1026,19 +1023,19 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
         <v>141</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1049,19 +1046,19 @@
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
         <v>139</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1072,19 +1069,19 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
         <v>137</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1095,26 +1092,26 @@
         <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1124,16 +1121,16 @@
         <v>14</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,16 +1141,16 @@
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
         <v>143</v>
       </c>
-      <c r="D12" t="s">
-        <v>144</v>
-      </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1167,16 +1164,16 @@
         <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1187,16 +1184,16 @@
         <v>17</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1207,48 +1204,48 @@
         <v>18</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" t="s">
         <v>115</v>
       </c>
-      <c r="D15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="A16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1256,48 +1253,48 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1305,45 +1302,45 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1351,77 +1348,77 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="7">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
         <v>21</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+      <c r="A27" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" t="s">
         <v>113</v>
-      </c>
-      <c r="D28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1429,19 +1426,19 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" s="7">
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1449,22 +1446,22 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" t="s">
         <v>117</v>
-      </c>
-      <c r="D30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1472,51 +1469,51 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="7">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
+      <c r="A32" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" t="s">
         <v>131</v>
       </c>
-      <c r="D33" t="s">
-        <v>132</v>
-      </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1524,51 +1521,51 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="7">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
+      <c r="A35" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" t="s">
         <v>129</v>
-      </c>
-      <c r="D36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1576,19 +1573,19 @@
         <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="7">
         <v>23</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37" t="s">
         <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1596,531 +1593,531 @@
         <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="7">
         <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
         <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="A39" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" s="7">
         <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" t="s">
         <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="7">
         <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E41" t="s">
         <v>21</v>
       </c>
       <c r="F41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C42" s="7">
         <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C43" s="7">
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E43" t="s">
         <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" t="s">
         <v>145</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D44" t="s">
-        <v>146</v>
-      </c>
       <c r="E44" t="s">
         <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C45" s="7">
         <v>62</v>
       </c>
       <c r="D45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E45" t="s">
         <v>21</v>
       </c>
       <c r="F45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C46" s="7">
         <v>61</v>
       </c>
       <c r="D46" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" t="s">
         <v>87</v>
-      </c>
-      <c r="E46" t="s">
-        <v>21</v>
-      </c>
-      <c r="F46" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C47" s="7">
         <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E47" t="s">
         <v>21</v>
       </c>
       <c r="F47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="15">
+        <v>144</v>
+      </c>
+      <c r="C48" s="13">
         <v>90</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C50" s="7">
         <v>84</v>
       </c>
       <c r="D50" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" t="s">
         <v>75</v>
-      </c>
-      <c r="E50" t="s">
-        <v>22</v>
-      </c>
-      <c r="F50" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C51" s="7">
         <v>77</v>
       </c>
       <c r="D51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" t="s">
         <v>78</v>
-      </c>
-      <c r="E51" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" s="7">
         <v>64</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C53" s="7">
         <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E53" t="s">
         <v>21</v>
       </c>
       <c r="F53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C54" s="7">
         <v>58</v>
       </c>
       <c r="D54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C55" s="7">
         <v>56</v>
       </c>
       <c r="F55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C56" s="7">
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C57" s="7">
         <v>53</v>
       </c>
       <c r="D57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E57" t="s">
         <v>21</v>
       </c>
       <c r="F57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C58" s="7">
         <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C59" s="7">
         <v>51</v>
       </c>
       <c r="F59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C60" s="7">
         <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C61" s="7">
         <v>36</v>
       </c>
       <c r="D61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" s="7">
         <v>32</v>
       </c>
       <c r="D62" t="s">
+        <v>101</v>
+      </c>
+      <c r="F62" t="s">
         <v>102</v>
       </c>
-      <c r="F62" t="s">
-        <v>103</v>
-      </c>
       <c r="G62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C63" s="7">
         <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="7">
         <v>29</v>
       </c>
       <c r="D64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C65" s="7">
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>